<commit_message>
Version 2.5.1 HighTypeChecker allow undefined as check value
</commit_message>
<xml_diff>
--- a/testcase/HighTypeChecker.xlsx
+++ b/testcase/HighTypeChecker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24345" windowHeight="12615"/>
+    <workbookView windowWidth="23925" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="TypeHighChecker" sheetId="2" r:id="rId1"/>
@@ -119,10 +119,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -133,6 +133,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -141,9 +186,56 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -164,7 +256,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,106 +264,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,187 +304,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,24 +509,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,6 +554,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -590,8 +590,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,10 +601,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -613,134 +613,134 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1235,17 +1235,22 @@
       <c r="C6">
         <v>1002</v>
       </c>
-      <c r="D6"/>
+      <c r="F6">
+        <v>2</v>
+      </c>
       <c r="G6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1257,6 +1262,9 @@
       </c>
       <c r="D8" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add high type checker 2.fix high type checker bug
</commit_message>
<xml_diff>
--- a/testcase/HighTypeChecker.xlsx
+++ b/testcase/HighTypeChecker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23925" windowHeight="12690" activeTab="2"/>
+    <workbookView windowWidth="24225" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="TypeHighChecker" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+  <si>
+    <t>#hight type checker example</t>
+  </si>
   <si>
     <t>AppType.ClientH |  AppType.ClientM | AppType.Gate | AppType.Logic</t>
   </si>
@@ -39,6 +42,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>#desc</t>
+  </si>
+  <si>
     <t>item</t>
   </si>
   <si>
@@ -57,6 +63,15 @@
     <t>itemlist</t>
   </si>
   <si>
+    <t>checkCell</t>
+  </si>
+  <si>
+    <t>checkCellSep</t>
+  </si>
+  <si>
+    <t>checkCellValue</t>
+  </si>
+  <si>
     <t>*int</t>
   </si>
   <si>
@@ -93,6 +108,12 @@
     <t>[Item.id][]</t>
   </si>
   <si>
+    <t>CheckGetCellData()</t>
+  </si>
+  <si>
+    <t>desc1</t>
+  </si>
+  <si>
     <t>1,10001,10000;2,1001,1</t>
   </si>
   <si>
@@ -102,7 +123,16 @@
     <t>10001,1;10002,1</t>
   </si>
   <si>
+    <t>desc2</t>
+  </si>
+  <si>
     <t>#3</t>
+  </si>
+  <si>
+    <t>desc3</t>
+  </si>
+  <si>
+    <t>desc4</t>
   </si>
   <si>
     <t>#Item Id</t>
@@ -122,10 +152,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -137,6 +167,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -144,7 +211,76 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,43 +294,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -205,76 +304,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,13 +337,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,169 +511,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,11 +533,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,35 +555,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,16 +595,36 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,10 +634,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -616,134 +646,134 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1106,174 +1136,250 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="16"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="16"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
         <v>10001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1001</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>101</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
         <v>10002</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1002</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>102</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>103</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9">
         <v>10003</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1003</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9">
         <v>2</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>104</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1295,34 +1401,34 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1457,8 +1563,8 @@
   <sheetPr/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1470,39 +1576,39 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1">

</xml_diff>